<commit_message>
🔁 Restaurando arquivos essenciais para deploy no Render
</commit_message>
<xml_diff>
--- a/dados/envios_log.xlsx
+++ b/dados/envios_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1021,10 +1021,8 @@
           <t>Ima Industria</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>04252502000160</t>
-        </is>
+      <c r="C24" t="n">
+        <v>4252502000160</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1034,6 +1032,83 @@
       <c r="E24" t="inlineStr">
         <is>
           <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>03/07/2025 16:31:04</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>4252502000160</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>03/07/2025 16:52:03</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>4252502000160</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>03/07/2025 16:52:12</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>RCD Educação</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>58475425000137</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>901-ExtratoMensal-052025.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
✅ Corrigido formato do Flask no requirements.txt
</commit_message>
<xml_diff>
--- a/dados/envios_log.xlsx
+++ b/dados/envios_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1096,10 +1096,8 @@
           <t>RCD Educação</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>58475425000137</t>
-        </is>
+      <c r="C27" t="n">
+        <v>58475425000137</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1109,6 +1107,33 @@
       <c r="E27" t="inlineStr">
         <is>
           <t>901-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>03/07/2025 17:08:13</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>04252502000160</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🧹 Limpeza de arquivos obsoletos e reorganização de estrutura
</commit_message>
<xml_diff>
--- a/dados/envios_log.xlsx
+++ b/dados/envios_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1121,10 +1121,8 @@
           <t>Ima Industria</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>04252502000160</t>
-        </is>
+      <c r="C28" t="n">
+        <v>4252502000160</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1134,6 +1132,108 @@
       <c r="E28" t="inlineStr">
         <is>
           <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>03/07/2025 21:40:09</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>4252502000160</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>03/07/2025 22:57:37</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>4252502000160</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>04/07/2025 11:20:05</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>4252502000160</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>04/07/2025 11:20:15</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>RCD Educação</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>58475425000137</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>901-ExtratoMensal-052025.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🧩 Torna rastreamento_leitura um pacote Python com __init__.py
</commit_message>
<xml_diff>
--- a/dados/envios_log.xlsx
+++ b/dados/envios_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1221,10 +1221,8 @@
           <t>RCD Educação</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>58475425000137</t>
-        </is>
+      <c r="C32" t="n">
+        <v>58475425000137</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1234,6 +1232,108 @@
       <c r="E32" t="inlineStr">
         <is>
           <t>901-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>04/07/2025 11:30:06</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>4252502000160</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>04/07/2025 11:30:15</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>RCD Educação</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>58475425000137</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>901-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>04/07/2025 12:48:38</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>4252502000160</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>04/07/2025 13:26:50</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>04252502000160</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔍 Adiciona logs de debug na rota /leituras
</commit_message>
<xml_diff>
--- a/dados/envios_log.xlsx
+++ b/dados/envios_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1321,17 +1321,42 @@
           <t>Ima Industria</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" t="n">
+        <v>4252502000160</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>893-ExtratoMensal-052025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>04/07/2025 17:26:42</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Ima Industria</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
         <is>
           <t>04252502000160</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>denissonfhsilva@gmail.com</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>denissonfhsilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>893-ExtratoMensal-052025.pdf</t>
         </is>

</xml_diff>